<commit_message>
changed Login.getCurrentUser() to GUI.getCurrentUser() to fix a bug when creating a new user and creating export/bankstatement
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt_bankstatement.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt_bankstatement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Category</t>
   </si>
@@ -27,6 +27,36 @@
   </si>
   <si>
     <t>Account</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>smed</t>
+  </si>
+  <si>
+    <t>2023-03-20</t>
+  </si>
+  <si>
+    <t>453.0</t>
+  </si>
+  <si>
+    <t>Checkings</t>
+  </si>
+  <si>
+    <t>buss</t>
+  </si>
+  <si>
+    <t>700.0</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>2023-03-22</t>
+  </si>
+  <si>
+    <t>1000.0</t>
   </si>
 </sst>
 </file>
@@ -71,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -94,6 +124,57 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>